<commit_message>
Adjusted Timetable to be from 9-6pm. Added constraint to prevent frequent scheduling of classes from 5-6pm
</commit_message>
<xml_diff>
--- a/data/NEWLY updated Timetable_Input_Template.xlsx
+++ b/data/NEWLY updated Timetable_Input_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamil\Downloads\SEPT 12\PAU_Timetable_Scheduler\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamil\Downloads\PAU_Timetable_Scheduler\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4842591-4188-4B67-B57E-77E94BEE892B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E67F9BD-28A4-4CD3-B425-E32C11DD8EDC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6804" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classrooms" sheetId="5" r:id="rId1"/>
@@ -3551,8 +3551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -3587,7 +3587,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -3601,7 +3601,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -3643,7 +3643,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -3657,7 +3657,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -3671,7 +3671,7 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -3685,7 +3685,7 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -3713,7 +3713,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
@@ -3727,7 +3727,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
@@ -3741,7 +3741,7 @@
         <v>5</v>
       </c>
       <c r="C13">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
@@ -3755,7 +3755,7 @@
         <v>5</v>
       </c>
       <c r="C14">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
         <v>18</v>
@@ -3783,7 +3783,7 @@
         <v>5</v>
       </c>
       <c r="C16">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
         <v>22</v>
@@ -3797,7 +3797,7 @@
         <v>5</v>
       </c>
       <c r="C17">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
         <v>22</v>
@@ -3811,7 +3811,7 @@
         <v>5</v>
       </c>
       <c r="C18">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
@@ -3839,7 +3839,7 @@
         <v>5</v>
       </c>
       <c r="C20">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -3853,7 +3853,7 @@
         <v>5</v>
       </c>
       <c r="C21">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
@@ -3881,7 +3881,7 @@
         <v>29</v>
       </c>
       <c r="C23">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -3895,7 +3895,7 @@
         <v>29</v>
       </c>
       <c r="C24">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -3909,7 +3909,7 @@
         <v>29</v>
       </c>
       <c r="C25">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D25" t="s">
         <v>22</v>
@@ -3923,7 +3923,7 @@
         <v>29</v>
       </c>
       <c r="C26">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D26" t="s">
         <v>34</v>
@@ -3937,7 +3937,7 @@
         <v>29</v>
       </c>
       <c r="C27">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D27" t="s">
         <v>36</v>
@@ -3951,7 +3951,7 @@
         <v>29</v>
       </c>
       <c r="C28">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
@@ -3965,7 +3965,7 @@
         <v>29</v>
       </c>
       <c r="C29">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
@@ -3979,7 +3979,7 @@
         <v>29</v>
       </c>
       <c r="C30">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D30" t="s">
         <v>22</v>
@@ -3993,7 +3993,7 @@
         <v>29</v>
       </c>
       <c r="C31">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D31" t="s">
         <v>41</v>
@@ -4007,7 +4007,7 @@
         <v>29</v>
       </c>
       <c r="C32">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D32" t="s">
         <v>43</v>
@@ -4021,7 +4021,7 @@
         <v>29</v>
       </c>
       <c r="C33">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D33" t="s">
         <v>6</v>
@@ -4035,7 +4035,7 @@
         <v>29</v>
       </c>
       <c r="C34">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D34" t="s">
         <v>6</v>
@@ -4049,7 +4049,7 @@
         <v>29</v>
       </c>
       <c r="C35">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D35" t="s">
         <v>6</v>
@@ -4063,7 +4063,7 @@
         <v>29</v>
       </c>
       <c r="C36">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
@@ -4091,7 +4091,7 @@
         <v>29</v>
       </c>
       <c r="C38">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="D38" t="s">
         <v>6</v>
@@ -7351,7 +7351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L285"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F276" sqref="F276"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adjusted Constraint Penalties and Bug Fixes
</commit_message>
<xml_diff>
--- a/data/NEWLY updated Timetable_Input_Template.xlsx
+++ b/data/NEWLY updated Timetable_Input_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamil\Downloads\PAU_Timetable_Scheduler\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B1C671-1AA8-4850-8A6F-B8E91BFFAAB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A17A3FA-A023-40D5-8970-FA136F5D2B82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6804" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6804" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classrooms" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3039" uniqueCount="1024">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3039" uniqueCount="1029">
   <si>
     <t>Room Name</t>
   </si>
@@ -3100,7 +3100,22 @@
     <t>uchegbuna@gmail.com</t>
   </si>
   <si>
-    <t>Thu</t>
+    <t>9:00-14:00</t>
+  </si>
+  <si>
+    <t>9:00-14:01</t>
+  </si>
+  <si>
+    <t>9:00-14:02</t>
+  </si>
+  <si>
+    <t>9:00-14:03</t>
+  </si>
+  <si>
+    <t>9:00-14:04</t>
+  </si>
+  <si>
+    <t>Tue, Wed, Thu</t>
   </si>
 </sst>
 </file>
@@ -5051,8 +5066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I136"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F137" sqref="F137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -6396,7 +6411,7 @@
         <v>1015</v>
       </c>
       <c r="F78" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -6413,7 +6428,7 @@
         <v>1017</v>
       </c>
       <c r="F79" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -6430,7 +6445,7 @@
         <v>1015</v>
       </c>
       <c r="F80" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -6447,7 +6462,7 @@
         <v>1017</v>
       </c>
       <c r="F81" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -6464,7 +6479,7 @@
         <v>1015</v>
       </c>
       <c r="F82" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -6481,7 +6496,7 @@
         <v>1017</v>
       </c>
       <c r="F83" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -6583,7 +6598,7 @@
         <v>1017</v>
       </c>
       <c r="F89" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -6600,7 +6615,7 @@
         <v>1015</v>
       </c>
       <c r="F90" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -6617,7 +6632,7 @@
         <v>1017</v>
       </c>
       <c r="F91" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -6634,7 +6649,7 @@
         <v>1015</v>
       </c>
       <c r="F92" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -6651,7 +6666,7 @@
         <v>1017</v>
       </c>
       <c r="F93" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -6702,7 +6717,7 @@
         <v>1015</v>
       </c>
       <c r="F96" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -6719,7 +6734,7 @@
         <v>1017</v>
       </c>
       <c r="F97" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -6770,7 +6785,7 @@
         <v>1015</v>
       </c>
       <c r="F100" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -6787,7 +6802,7 @@
         <v>1017</v>
       </c>
       <c r="F101" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -6804,7 +6819,7 @@
         <v>1015</v>
       </c>
       <c r="F102" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -6821,7 +6836,7 @@
         <v>1017</v>
       </c>
       <c r="F103" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -6940,7 +6955,7 @@
         <v>1015</v>
       </c>
       <c r="F110" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -6957,7 +6972,7 @@
         <v>1017</v>
       </c>
       <c r="F111" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -6974,7 +6989,7 @@
         <v>1015</v>
       </c>
       <c r="F112" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -6991,7 +7006,7 @@
         <v>1017</v>
       </c>
       <c r="F113" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -7008,7 +7023,7 @@
         <v>1015</v>
       </c>
       <c r="F114" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -7025,7 +7040,7 @@
         <v>1017</v>
       </c>
       <c r="F115" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -7127,7 +7142,7 @@
         <v>1017</v>
       </c>
       <c r="F121" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -7144,7 +7159,7 @@
         <v>1015</v>
       </c>
       <c r="F122" t="s">
-        <v>1014</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -7161,7 +7176,7 @@
         <v>1017</v>
       </c>
       <c r="F123" t="s">
-        <v>1014</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -7178,7 +7193,7 @@
         <v>1015</v>
       </c>
       <c r="F124" t="s">
-        <v>1014</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -7195,7 +7210,7 @@
         <v>1017</v>
       </c>
       <c r="F125" t="s">
-        <v>1014</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -7229,7 +7244,7 @@
         <v>1017</v>
       </c>
       <c r="F127" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -7263,7 +7278,7 @@
         <v>1017</v>
       </c>
       <c r="F129" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -7297,7 +7312,7 @@
         <v>1017</v>
       </c>
       <c r="F131" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -7314,7 +7329,7 @@
         <v>1015</v>
       </c>
       <c r="F132" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -7331,7 +7346,7 @@
         <v>1017</v>
       </c>
       <c r="F133" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -7348,7 +7363,7 @@
         <v>1015</v>
       </c>
       <c r="F134" t="s">
-        <v>1014</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -7379,7 +7394,7 @@
         <v>210</v>
       </c>
       <c r="E136" t="s">
-        <v>1023</v>
+        <v>1028</v>
       </c>
       <c r="F136" t="s">
         <v>1013</v>
@@ -7419,7 +7434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+    <sheetView topLeftCell="A95" workbookViewId="0">
       <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>

</xml_diff>